<commit_message>
Pull July 2024 data
</commit_message>
<xml_diff>
--- a/reports/data.xlsx
+++ b/reports/data.xlsx
@@ -17,10 +17,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -39,6 +39,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -48,21 +55,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -70,7 +70,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -85,6 +85,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -93,7 +101,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -101,13 +109,50 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -124,7 +169,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -137,51 +182,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -192,181 +192,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -389,8 +389,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -399,7 +399,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -419,21 +419,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -445,6 +430,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -467,19 +463,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -488,152 +488,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="6">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="3">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="3">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="3">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="3">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="4">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0">
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="8">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -645,7 +645,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -974,7 +973,7 @@
   <dimension ref="A1:C104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="$A1:$XFD1048576"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -988,9 +987,10 @@
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
+      <c r="C2"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2"/>
@@ -1004,112 +1004,116 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="4"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="7"/>
+      <c r="A6" s="6"/>
       <c r="B6"/>
       <c r="C6"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="7"/>
+      <c r="A7" s="6"/>
       <c r="B7"/>
       <c r="C7"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="7"/>
+      <c r="A8" s="6"/>
       <c r="B8"/>
       <c r="C8"/>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="7"/>
+      <c r="A9" s="6"/>
       <c r="B9"/>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="7"/>
+      <c r="A10" s="6"/>
       <c r="B10"/>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="7"/>
+      <c r="A11" s="6"/>
       <c r="B11"/>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="7"/>
+    <row r="12" spans="1:3">
+      <c r="A12" s="6"/>
       <c r="B12"/>
+      <c r="C12"/>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="7"/>
+      <c r="A13" s="6"/>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="7"/>
+      <c r="A14" s="6"/>
       <c r="B14"/>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="7"/>
+      <c r="A15" s="6"/>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="7"/>
+      <c r="A16" s="6"/>
       <c r="B16"/>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="7"/>
+      <c r="A17" s="6"/>
       <c r="B17"/>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="7"/>
+    <row r="18" spans="1:3">
+      <c r="A18" s="6"/>
       <c r="B18"/>
+      <c r="C18"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="7"/>
+      <c r="A19" s="6"/>
       <c r="B19"/>
       <c r="C19"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="4"/>
-      <c r="B20" s="6"/>
+      <c r="B20" s="5"/>
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="4"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="7"/>
+      <c r="A22" s="6"/>
       <c r="B22"/>
       <c r="C22"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="7"/>
+      <c r="A23" s="6"/>
       <c r="B23"/>
       <c r="C23"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="7"/>
+      <c r="A24" s="6"/>
       <c r="B24"/>
       <c r="C24"/>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="7"/>
+      <c r="A25" s="6"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="7"/>
+      <c r="A26" s="6"/>
       <c r="B26"/>
       <c r="C26"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="7"/>
+      <c r="A27" s="6"/>
       <c r="B27"/>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="7"/>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="7"/>
+      <c r="A28" s="6"/>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="6"/>
+      <c r="B29"/>
+      <c r="C29"/>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="7"/>
+      <c r="A30" s="6"/>
       <c r="B30"/>
       <c r="C30"/>
     </row>
@@ -1120,43 +1124,45 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="4"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="7"/>
+      <c r="A33" s="6"/>
       <c r="B33"/>
       <c r="C33"/>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="7"/>
+      <c r="A34" s="6"/>
       <c r="B34"/>
       <c r="C34"/>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="7"/>
+      <c r="A35" s="6"/>
       <c r="B35"/>
       <c r="C35"/>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="7"/>
+      <c r="A36" s="6"/>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="7"/>
+      <c r="A37" s="6"/>
       <c r="C37"/>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="7"/>
+      <c r="A38" s="6"/>
       <c r="B38"/>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="7"/>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="7"/>
+      <c r="A39" s="6"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="6"/>
+      <c r="B40"/>
+      <c r="C40"/>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="7"/>
+      <c r="A41" s="6"/>
       <c r="B41"/>
       <c r="C41"/>
     </row>
@@ -1167,36 +1173,37 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="4"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="7"/>
+      <c r="A44" s="6"/>
       <c r="B44"/>
       <c r="C44"/>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="7"/>
+      <c r="A45" s="6"/>
       <c r="B45"/>
       <c r="C45"/>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="7"/>
+      <c r="A46" s="6"/>
       <c r="C46"/>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="7"/>
+      <c r="A47" s="6"/>
       <c r="C47"/>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="7"/>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="7"/>
+      <c r="A48" s="6"/>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="6"/>
       <c r="B49"/>
+      <c r="C49"/>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="7"/>
+      <c r="A50" s="6"/>
       <c r="B50"/>
       <c r="C50"/>
     </row>
@@ -1207,39 +1214,41 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="4"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="7"/>
+      <c r="A53" s="6"/>
       <c r="B53"/>
       <c r="C53"/>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="7"/>
+      <c r="A54" s="6"/>
       <c r="B54"/>
       <c r="C54"/>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="7"/>
+      <c r="A55" s="6"/>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="7"/>
+      <c r="A56" s="6"/>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" s="7"/>
+      <c r="A57" s="6"/>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="7"/>
+      <c r="A58" s="6"/>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="7"/>
-    </row>
-    <row r="60" spans="1:1">
-      <c r="A60" s="7"/>
+      <c r="A59" s="6"/>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="6"/>
+      <c r="B60"/>
+      <c r="C60"/>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="7"/>
+      <c r="A61" s="6"/>
       <c r="B61"/>
       <c r="C61"/>
     </row>
@@ -1250,41 +1259,43 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="4"/>
-      <c r="B63" s="6"/>
-      <c r="C63" s="6"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="7"/>
+      <c r="A64" s="6"/>
       <c r="B64"/>
       <c r="C64"/>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="7"/>
+      <c r="A65" s="6"/>
       <c r="B65"/>
       <c r="C65"/>
     </row>
     <row r="66" spans="1:1">
-      <c r="A66" s="7"/>
+      <c r="A66" s="6"/>
     </row>
     <row r="67" spans="1:1">
-      <c r="A67" s="7"/>
+      <c r="A67" s="6"/>
     </row>
     <row r="68" spans="1:2">
-      <c r="A68" s="7"/>
+      <c r="A68" s="6"/>
       <c r="B68"/>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" s="7"/>
+      <c r="A69" s="6"/>
       <c r="C69"/>
     </row>
     <row r="70" spans="1:1">
-      <c r="A70" s="7"/>
-    </row>
-    <row r="71" spans="1:1">
-      <c r="A71" s="7"/>
+      <c r="A70" s="6"/>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="6"/>
+      <c r="B71"/>
+      <c r="C71"/>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="7"/>
+      <c r="A72" s="6"/>
       <c r="B72"/>
       <c r="C72"/>
     </row>
@@ -1295,27 +1306,29 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="4"/>
-      <c r="B74" s="6"/>
-      <c r="C74" s="6"/>
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="7"/>
+      <c r="A75" s="6"/>
       <c r="B75"/>
       <c r="C75"/>
     </row>
     <row r="76" spans="1:3">
-      <c r="A76" s="7"/>
+      <c r="A76" s="6"/>
       <c r="B76"/>
       <c r="C76"/>
     </row>
     <row r="77" spans="1:1">
-      <c r="A77" s="7"/>
-    </row>
-    <row r="78" spans="1:1">
-      <c r="A78" s="7"/>
+      <c r="A77" s="6"/>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="6"/>
+      <c r="B78"/>
+      <c r="C78"/>
     </row>
     <row r="79" spans="1:3">
-      <c r="A79" s="7"/>
+      <c r="A79" s="6"/>
       <c r="B79"/>
       <c r="C79"/>
     </row>
@@ -1326,54 +1339,56 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="4"/>
-      <c r="B81" s="6"/>
-      <c r="C81" s="6"/>
+      <c r="B81" s="5"/>
+      <c r="C81" s="5"/>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" s="7"/>
+      <c r="A82" s="6"/>
       <c r="B82"/>
       <c r="C82"/>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" s="7"/>
+      <c r="A83" s="6"/>
       <c r="B83"/>
       <c r="C83"/>
     </row>
     <row r="84" spans="1:2">
-      <c r="A84" s="7"/>
+      <c r="A84" s="6"/>
       <c r="B84"/>
     </row>
     <row r="85" spans="1:2">
-      <c r="A85" s="7"/>
+      <c r="A85" s="6"/>
       <c r="B85"/>
     </row>
     <row r="86" spans="1:3">
-      <c r="A86" s="7"/>
+      <c r="A86" s="6"/>
       <c r="B86"/>
       <c r="C86"/>
     </row>
     <row r="87" spans="1:3">
-      <c r="A87" s="7"/>
+      <c r="A87" s="6"/>
       <c r="C87"/>
     </row>
     <row r="88" spans="1:3">
-      <c r="A88" s="7"/>
+      <c r="A88" s="6"/>
       <c r="C88"/>
     </row>
     <row r="89" spans="1:1">
-      <c r="A89" s="7"/>
+      <c r="A89" s="6"/>
     </row>
     <row r="90" spans="1:1">
-      <c r="A90" s="7"/>
+      <c r="A90" s="6"/>
     </row>
     <row r="91" spans="1:1">
-      <c r="A91" s="7"/>
-    </row>
-    <row r="92" spans="1:1">
-      <c r="A92" s="7"/>
+      <c r="A91" s="6"/>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="6"/>
+      <c r="B92"/>
+      <c r="C92"/>
     </row>
     <row r="93" spans="1:3">
-      <c r="A93" s="7"/>
+      <c r="A93" s="6"/>
       <c r="B93"/>
       <c r="C93"/>
     </row>
@@ -1384,40 +1399,40 @@
     </row>
     <row r="95" spans="1:3">
       <c r="A95" s="4"/>
-      <c r="B95" s="6"/>
-      <c r="C95" s="6"/>
+      <c r="B95" s="5"/>
+      <c r="C95" s="5"/>
     </row>
     <row r="96" spans="1:3">
-      <c r="A96" s="7"/>
+      <c r="A96" s="6"/>
       <c r="B96"/>
       <c r="C96"/>
     </row>
     <row r="97" spans="1:3">
-      <c r="A97" s="7"/>
+      <c r="A97" s="6"/>
       <c r="B97"/>
       <c r="C97"/>
     </row>
     <row r="98" spans="1:3">
-      <c r="A98" s="7"/>
+      <c r="A98" s="6"/>
       <c r="B98"/>
       <c r="C98"/>
     </row>
     <row r="99" spans="1:3">
-      <c r="A99" s="7"/>
+      <c r="A99" s="6"/>
       <c r="C99"/>
     </row>
     <row r="100" spans="1:3">
-      <c r="A100" s="7"/>
+      <c r="A100" s="6"/>
       <c r="B100"/>
       <c r="C100"/>
     </row>
     <row r="101" spans="1:3">
-      <c r="A101" s="7"/>
+      <c r="A101" s="6"/>
       <c r="B101"/>
       <c r="C101"/>
     </row>
     <row r="102" spans="1:3">
-      <c r="A102" s="7"/>
+      <c r="A102" s="6"/>
       <c r="C102"/>
     </row>
     <row r="103" spans="1:1">
@@ -1435,10 +1450,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C103"/>
+  <dimension ref="A1:C108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="54" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -1460,136 +1475,138 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
+      <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="4"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="7"/>
+      <c r="A5" s="6"/>
       <c r="B5"/>
       <c r="C5"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="7"/>
+      <c r="A6" s="6"/>
       <c r="B6"/>
       <c r="C6"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="7"/>
+      <c r="A7" s="6"/>
       <c r="B7"/>
       <c r="C7"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="7"/>
+      <c r="A8" s="6"/>
       <c r="B8"/>
       <c r="C8"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="7"/>
+      <c r="A9" s="6"/>
       <c r="B9"/>
       <c r="C9"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="7"/>
+      <c r="A10" s="6"/>
       <c r="B10"/>
       <c r="C10"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="7"/>
+      <c r="A11" s="6"/>
       <c r="B11"/>
       <c r="C11"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="7"/>
+      <c r="A12" s="6"/>
       <c r="B12"/>
       <c r="C12"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="7"/>
+      <c r="A13" s="6"/>
       <c r="B13"/>
       <c r="C13"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="7"/>
+      <c r="A14" s="6"/>
       <c r="B14"/>
       <c r="C14"/>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="7"/>
+      <c r="A15" s="6"/>
       <c r="B15"/>
       <c r="C15"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="7"/>
+      <c r="A16" s="6"/>
       <c r="B16"/>
       <c r="C16"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="7"/>
+      <c r="A17" s="6"/>
       <c r="B17"/>
       <c r="C17"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="7"/>
+      <c r="A18" s="6"/>
       <c r="B18"/>
       <c r="C18"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="4"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="4"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="7"/>
+      <c r="A21" s="6"/>
       <c r="B21"/>
       <c r="C21"/>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="7"/>
+      <c r="A22" s="6"/>
       <c r="B22"/>
       <c r="C22"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="7"/>
+      <c r="A23" s="6"/>
       <c r="B23"/>
       <c r="C23"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="7"/>
+      <c r="A24" s="6"/>
       <c r="B24"/>
       <c r="C24"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="7"/>
+      <c r="A25" s="6"/>
       <c r="B25"/>
       <c r="C25"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="7"/>
+      <c r="A26" s="6"/>
       <c r="B26"/>
       <c r="C26"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="7"/>
+      <c r="A27" s="6"/>
       <c r="B27"/>
       <c r="C27"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="7"/>
+      <c r="A28" s="6"/>
       <c r="B28"/>
       <c r="C28"/>
     </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="7"/>
+    <row r="29" spans="1:3">
+      <c r="A29" s="6"/>
+      <c r="B29"/>
+      <c r="C29"/>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="4"/>
@@ -1598,151 +1615,151 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="4"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="7"/>
+      <c r="A32" s="6"/>
       <c r="B32"/>
       <c r="C32"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="7"/>
+      <c r="A33" s="6"/>
       <c r="B33"/>
       <c r="C33"/>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="7"/>
+      <c r="A34" s="6"/>
       <c r="B34"/>
       <c r="C34"/>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="7"/>
+      <c r="A35" s="6"/>
       <c r="B35"/>
       <c r="C35"/>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="7"/>
+      <c r="A36" s="6"/>
       <c r="B36"/>
       <c r="C36"/>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="7"/>
+      <c r="A37" s="6"/>
       <c r="B37"/>
       <c r="C37"/>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="7"/>
+      <c r="A38" s="6"/>
       <c r="B38"/>
       <c r="C38"/>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="7"/>
+      <c r="A39" s="6"/>
       <c r="B39"/>
       <c r="C39"/>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="7"/>
+      <c r="A40" s="6"/>
       <c r="B40"/>
       <c r="C40"/>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="4"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="4"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="7"/>
+      <c r="A43" s="6"/>
       <c r="B43"/>
       <c r="C43"/>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="7"/>
+      <c r="A44" s="6"/>
       <c r="B44"/>
       <c r="C44"/>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="7"/>
+      <c r="A45" s="6"/>
       <c r="B45"/>
       <c r="C45"/>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="7"/>
+      <c r="A46" s="6"/>
       <c r="B46"/>
       <c r="C46"/>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="7"/>
+      <c r="A47" s="6"/>
       <c r="B47"/>
       <c r="C47"/>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="7"/>
+      <c r="A48" s="6"/>
       <c r="B48"/>
       <c r="C48"/>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="7"/>
+      <c r="A49" s="6"/>
       <c r="B49"/>
       <c r="C49"/>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="4"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="4"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="7"/>
+      <c r="A52" s="6"/>
       <c r="B52"/>
       <c r="C52"/>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="7"/>
+      <c r="A53" s="6"/>
       <c r="B53"/>
       <c r="C53"/>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="7"/>
+      <c r="A54" s="6"/>
       <c r="B54"/>
       <c r="C54"/>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="7"/>
+      <c r="A55" s="6"/>
       <c r="B55"/>
       <c r="C55"/>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="7"/>
+      <c r="A56" s="6"/>
       <c r="B56"/>
       <c r="C56"/>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="7"/>
+      <c r="A57" s="6"/>
       <c r="B57"/>
       <c r="C57"/>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" s="7"/>
+      <c r="A58" s="6"/>
       <c r="B58"/>
       <c r="C58"/>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="7"/>
+      <c r="A59" s="6"/>
       <c r="B59"/>
       <c r="C59"/>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="7"/>
+      <c r="A60" s="6"/>
       <c r="B60"/>
       <c r="C60"/>
     </row>
@@ -1753,209 +1770,236 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="4"/>
-      <c r="B62" s="6"/>
-      <c r="C62" s="6"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="7"/>
+      <c r="A63" s="6"/>
       <c r="B63"/>
       <c r="C63"/>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="7"/>
+      <c r="A64" s="6"/>
       <c r="B64"/>
       <c r="C64"/>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="7"/>
+      <c r="A65" s="6"/>
       <c r="B65"/>
       <c r="C65"/>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="7"/>
+      <c r="A66" s="6"/>
       <c r="B66"/>
       <c r="C66"/>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="7"/>
+      <c r="A67" s="6"/>
       <c r="B67"/>
       <c r="C67"/>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" s="7"/>
+      <c r="A68" s="6"/>
       <c r="B68"/>
       <c r="C68"/>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" s="7"/>
+      <c r="A69" s="6"/>
       <c r="B69"/>
       <c r="C69"/>
     </row>
     <row r="70" spans="1:2">
-      <c r="A70" s="7"/>
+      <c r="A70" s="6"/>
       <c r="B70"/>
     </row>
-    <row r="71" spans="1:1">
-      <c r="A71" s="7"/>
+    <row r="71" spans="1:3">
+      <c r="A71" s="6"/>
+      <c r="B71"/>
+      <c r="C71"/>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="4"/>
-      <c r="B72" s="6"/>
-      <c r="C72" s="6"/>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="4"/>
-      <c r="B73" s="6"/>
-      <c r="C73" s="6"/>
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="7"/>
+      <c r="A74" s="6"/>
       <c r="B74"/>
       <c r="C74"/>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="7"/>
+      <c r="A75" s="6"/>
       <c r="B75"/>
       <c r="C75"/>
     </row>
     <row r="76" spans="1:3">
-      <c r="A76" s="7"/>
+      <c r="A76" s="6"/>
       <c r="B76"/>
       <c r="C76"/>
     </row>
     <row r="77" spans="1:2">
-      <c r="A77" s="7"/>
+      <c r="A77" s="6"/>
       <c r="B77"/>
     </row>
     <row r="78" spans="1:3">
-      <c r="A78" s="7"/>
+      <c r="A78" s="6"/>
       <c r="B78"/>
       <c r="C78"/>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="4"/>
-      <c r="B79" s="6"/>
-      <c r="C79" s="6"/>
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="4"/>
-      <c r="B80" s="6"/>
-      <c r="C80" s="6"/>
+      <c r="B80" s="5"/>
+      <c r="C80" s="5"/>
     </row>
     <row r="81" spans="1:3">
-      <c r="A81" s="7"/>
+      <c r="A81" s="6"/>
       <c r="B81"/>
       <c r="C81"/>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" s="7"/>
+      <c r="A82" s="6"/>
       <c r="B82"/>
       <c r="C82"/>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" s="7"/>
+      <c r="A83" s="6"/>
       <c r="B83"/>
       <c r="C83"/>
     </row>
     <row r="84" spans="1:3">
-      <c r="A84" s="7"/>
+      <c r="A84" s="6"/>
       <c r="B84"/>
       <c r="C84"/>
     </row>
     <row r="85" spans="1:3">
-      <c r="A85" s="7"/>
+      <c r="A85" s="6"/>
       <c r="B85"/>
       <c r="C85"/>
     </row>
     <row r="86" spans="1:3">
-      <c r="A86" s="7"/>
+      <c r="A86" s="6"/>
       <c r="B86"/>
       <c r="C86"/>
     </row>
     <row r="87" spans="1:3">
-      <c r="A87" s="7"/>
+      <c r="A87" s="6"/>
       <c r="B87"/>
       <c r="C87"/>
     </row>
     <row r="88" spans="1:3">
-      <c r="A88" s="7"/>
+      <c r="A88" s="6"/>
       <c r="B88"/>
       <c r="C88"/>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89" s="7"/>
+      <c r="A89" s="6"/>
       <c r="B89"/>
       <c r="C89"/>
     </row>
     <row r="90" spans="1:3">
-      <c r="A90" s="7"/>
+      <c r="A90" s="6"/>
       <c r="B90"/>
       <c r="C90"/>
     </row>
     <row r="91" spans="1:3">
-      <c r="A91" s="7"/>
+      <c r="A91" s="6"/>
       <c r="B91"/>
       <c r="C91"/>
     </row>
     <row r="92" spans="1:3">
-      <c r="A92" s="7"/>
+      <c r="A92" s="6"/>
       <c r="B92"/>
       <c r="C92"/>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" s="4"/>
       <c r="B93" s="2"/>
-      <c r="C93" s="6"/>
+      <c r="C93" s="5"/>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" s="4"/>
-      <c r="B94" s="6"/>
-      <c r="C94" s="6"/>
+      <c r="B94" s="5"/>
+      <c r="C94" s="5"/>
     </row>
     <row r="95" spans="1:3">
-      <c r="A95" s="7"/>
+      <c r="A95" s="6"/>
       <c r="B95"/>
       <c r="C95"/>
     </row>
     <row r="96" spans="1:3">
-      <c r="A96" s="7"/>
+      <c r="A96" s="6"/>
       <c r="B96"/>
       <c r="C96"/>
     </row>
     <row r="97" spans="1:3">
-      <c r="A97" s="7"/>
+      <c r="A97" s="6"/>
       <c r="B97"/>
       <c r="C97"/>
     </row>
     <row r="98" spans="1:3">
-      <c r="A98" s="7"/>
+      <c r="A98" s="6"/>
       <c r="B98"/>
       <c r="C98"/>
     </row>
     <row r="99" spans="1:3">
-      <c r="A99" s="7"/>
+      <c r="A99" s="6"/>
       <c r="B99"/>
       <c r="C99"/>
     </row>
     <row r="100" spans="1:3">
-      <c r="A100" s="7"/>
+      <c r="A100" s="6"/>
       <c r="B100"/>
       <c r="C100"/>
     </row>
     <row r="101" spans="1:3">
-      <c r="A101" s="7"/>
+      <c r="A101" s="6"/>
       <c r="B101"/>
       <c r="C101"/>
     </row>
     <row r="102" spans="1:3">
-      <c r="A102"/>
+      <c r="A102" s="6"/>
       <c r="B102"/>
       <c r="C102"/>
     </row>
     <row r="103" spans="1:3">
-      <c r="A103"/>
-      <c r="B103"/>
-      <c r="C103"/>
+      <c r="A103" s="4"/>
+      <c r="B103" s="5"/>
+      <c r="C103" s="5"/>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="4"/>
+      <c r="B104" s="5"/>
+      <c r="C104" s="5"/>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="6"/>
+      <c r="B105"/>
+      <c r="C105"/>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="6"/>
+      <c r="B106"/>
+      <c r="C106"/>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="6"/>
+      <c r="B107"/>
+      <c r="C107"/>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="6"/>
+      <c r="B108"/>
+      <c r="C108"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>